<commit_message>
adding hyperlinks and more datasets
</commit_message>
<xml_diff>
--- a/primary_literature/TOC.xlsx
+++ b/primary_literature/TOC.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Shockwing/Dropbox/Boston/phd/repos/dnadesign-data/primary_literature/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6B8B5B5-7312-E146-A277-95C8EE050BBA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2474378D-B4B7-0F46-935E-DEF3468510BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17860" xr2:uid="{84B45C76-4322-224B-B312-91E503F65D31}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="230" uniqueCount="210">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="235" uniqueCount="215">
   <si>
     <t>comments</t>
   </si>
@@ -666,6 +666,21 @@
   </si>
   <si>
     <t>Lu et al. performed a transcriptome analysis of E. coli exposed to 200 mM glyphosate identified the differential expression of 1040 genes, which represent 23.2% of the genome</t>
+  </si>
+  <si>
+    <t>Deter et al</t>
+  </si>
+  <si>
+    <t>Antibiotic tolerance is associated with a broad and complex transcriptional response in E. coli</t>
+  </si>
+  <si>
+    <t>10.1038/s41598-021-85509-7</t>
+  </si>
+  <si>
+    <t>Ampicillin resistance</t>
+  </si>
+  <si>
+    <t>Deter et al. generated RNA-seq data on both antibiotic-treated and -untreated populations emerging from stationary phase.</t>
   </si>
 </sst>
 </file>
@@ -1031,9 +1046,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{84F68783-878B-3345-9072-70C5BAEE55D7}">
-  <dimension ref="A1:E46"/>
+  <dimension ref="A1:E47"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C30" sqref="C30"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -1128,698 +1145,715 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
-        <v>73</v>
+        <v>210</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>70</v>
+        <v>211</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>72</v>
+        <v>212</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>20</v>
+        <v>213</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>71</v>
+        <v>214</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
-        <v>158</v>
+        <v>73</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>157</v>
+        <v>70</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>156</v>
+        <v>72</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>159</v>
+        <v>20</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>160</v>
+        <v>71</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
-        <v>56</v>
+        <v>158</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>52</v>
+        <v>157</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>55</v>
+        <v>156</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>53</v>
+        <v>159</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>54</v>
+        <v>160</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
-        <v>41</v>
+        <v>56</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>42</v>
+        <v>52</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>40</v>
+        <v>55</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>20</v>
+        <v>53</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>39</v>
+        <v>54</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
-        <v>115</v>
+        <v>41</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>116</v>
+        <v>42</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>117</v>
+        <v>40</v>
       </c>
       <c r="D10" s="1" t="s">
         <v>20</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>118</v>
+        <v>39</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
-        <v>123</v>
+        <v>115</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>124</v>
+        <v>116</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>125</v>
+        <v>117</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>137</v>
+        <v>20</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>126</v>
+        <v>118</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
-        <v>6</v>
+        <v>123</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>5</v>
+        <v>124</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>9</v>
+        <v>125</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>7</v>
+        <v>137</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>8</v>
+        <v>126</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
-        <v>80</v>
+        <v>6</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>78</v>
+        <v>5</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>79</v>
+        <v>9</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>20</v>
+        <v>7</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>81</v>
+        <v>8</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
-        <v>111</v>
+        <v>80</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>110</v>
+        <v>78</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>113</v>
+        <v>79</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>112</v>
+        <v>20</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>114</v>
+        <v>81</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
-        <v>185</v>
+        <v>111</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>183</v>
+        <v>110</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>184</v>
+        <v>113</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>176</v>
+        <v>112</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>186</v>
+        <v>114</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
-        <v>23</v>
+        <v>185</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>19</v>
+        <v>183</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>22</v>
+        <v>184</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>20</v>
+        <v>176</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>21</v>
+        <v>186</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
-        <v>122</v>
+        <v>23</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>119</v>
+        <v>19</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>120</v>
+        <v>22</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>112</v>
+        <v>20</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>121</v>
+        <v>21</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
-        <v>187</v>
+        <v>122</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>188</v>
+        <v>119</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>189</v>
+        <v>120</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>190</v>
+        <v>112</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>191</v>
+        <v>121</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
+        <v>187</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A20" s="1" t="s">
         <v>202</v>
       </c>
-      <c r="B19" s="1" t="s">
+      <c r="B20" s="1" t="s">
         <v>203</v>
       </c>
-      <c r="C19" s="1" t="s">
+      <c r="C20" s="1" t="s">
         <v>204</v>
       </c>
-      <c r="D19" s="1" t="s">
+      <c r="D20" s="1" t="s">
         <v>195</v>
       </c>
-      <c r="E19" s="1" t="s">
+      <c r="E20" s="1" t="s">
         <v>205</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A20" s="2" t="s">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A21" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B20" s="2" t="s">
+      <c r="B21" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="C20" s="2" t="s">
+      <c r="C21" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="D20" s="2" t="s">
+      <c r="D21" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="E20" s="2" t="s">
+      <c r="E21" s="2" t="s">
         <v>11</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A21" s="1" t="s">
-        <v>181</v>
-      </c>
-      <c r="B21" s="1" t="s">
-        <v>179</v>
-      </c>
-      <c r="C21" s="1" t="s">
-        <v>180</v>
-      </c>
-      <c r="D21" s="1" t="s">
-        <v>176</v>
-      </c>
-      <c r="E21" s="1" t="s">
-        <v>182</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
-        <v>38</v>
+        <v>181</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>34</v>
+        <v>179</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>37</v>
+        <v>180</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>35</v>
+        <v>176</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>36</v>
+        <v>182</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
-        <v>151</v>
+        <v>38</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>152</v>
+        <v>34</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>153</v>
+        <v>37</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>154</v>
+        <v>35</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>155</v>
+        <v>36</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
-        <v>51</v>
+        <v>151</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>47</v>
+        <v>152</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>50</v>
+        <v>153</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>48</v>
+        <v>154</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>49</v>
+        <v>155</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
-        <v>206</v>
+        <v>51</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>207</v>
+        <v>47</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>208</v>
+        <v>50</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>20</v>
+        <v>48</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>209</v>
+        <v>49</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
-        <v>105</v>
+        <v>206</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>109</v>
+        <v>207</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>108</v>
+        <v>208</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>106</v>
+        <v>20</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>107</v>
+        <v>209</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="s">
-        <v>69</v>
+        <v>105</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>66</v>
+        <v>109</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>68</v>
+        <v>108</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>58</v>
+        <v>106</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>67</v>
+        <v>107</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A28" s="1" t="s">
-        <v>65</v>
+        <v>69</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>64</v>
+        <v>68</v>
       </c>
       <c r="D28" s="1" t="s">
         <v>58</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>63</v>
+        <v>67</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A29" s="1" t="s">
-        <v>61</v>
+        <v>65</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>57</v>
+        <v>62</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="D29" s="1" t="s">
         <v>58</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A30" s="1" t="s">
-        <v>46</v>
+        <v>61</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>43</v>
+        <v>57</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>45</v>
+        <v>60</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>28</v>
+        <v>58</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>44</v>
+        <v>59</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A31" s="1" t="s">
-        <v>147</v>
+        <v>46</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>148</v>
+        <v>43</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>149</v>
+        <v>45</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>20</v>
+        <v>28</v>
       </c>
       <c r="E31" s="1" t="s">
-        <v>150</v>
+        <v>44</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A32" s="1" t="s">
-        <v>161</v>
+        <v>147</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>162</v>
+        <v>148</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>163</v>
+        <v>149</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>141</v>
+        <v>20</v>
       </c>
       <c r="E32" s="1" t="s">
-        <v>164</v>
+        <v>150</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A33" s="1" t="s">
-        <v>96</v>
+        <v>161</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>99</v>
+        <v>162</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>98</v>
+        <v>163</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>20</v>
+        <v>141</v>
       </c>
       <c r="E33" s="1" t="s">
-        <v>97</v>
+        <v>164</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A34" s="1" t="s">
-        <v>127</v>
+        <v>96</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>128</v>
+        <v>99</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>133</v>
+        <v>98</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>129</v>
+        <v>20</v>
       </c>
       <c r="E34" s="1" t="s">
-        <v>130</v>
+        <v>97</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A35" s="1" t="s">
-        <v>100</v>
+        <v>127</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>104</v>
+        <v>128</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>103</v>
+        <v>133</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>101</v>
+        <v>129</v>
       </c>
       <c r="E35" s="1" t="s">
-        <v>102</v>
+        <v>130</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A36" s="1" t="s">
-        <v>143</v>
+        <v>100</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>144</v>
+        <v>104</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>145</v>
+        <v>103</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>112</v>
+        <v>101</v>
       </c>
       <c r="E36" s="1" t="s">
-        <v>146</v>
+        <v>102</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A37" s="1" t="s">
-        <v>95</v>
+        <v>143</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>91</v>
+        <v>144</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>92</v>
+        <v>145</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>93</v>
+        <v>112</v>
       </c>
       <c r="E37" s="1" t="s">
-        <v>94</v>
+        <v>146</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A38" s="1" t="s">
-        <v>33</v>
+        <v>95</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>30</v>
+        <v>91</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>32</v>
+        <v>92</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>20</v>
+        <v>93</v>
       </c>
       <c r="E38" s="1" t="s">
-        <v>31</v>
+        <v>94</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A39" s="1" t="s">
-        <v>178</v>
+        <v>33</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>174</v>
+        <v>30</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>175</v>
+        <v>32</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>176</v>
+        <v>20</v>
       </c>
       <c r="E39" s="1" t="s">
-        <v>177</v>
+        <v>31</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A40" s="1" t="s">
-        <v>197</v>
+        <v>178</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>198</v>
+        <v>174</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>199</v>
+        <v>175</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>200</v>
+        <v>176</v>
       </c>
       <c r="E40" s="1" t="s">
-        <v>201</v>
+        <v>177</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A41" s="1" t="s">
-        <v>88</v>
+        <v>197</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>86</v>
+        <v>198</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>87</v>
+        <v>199</v>
       </c>
       <c r="D41" s="1" t="s">
-        <v>90</v>
+        <v>200</v>
       </c>
       <c r="E41" s="1" t="s">
-        <v>89</v>
+        <v>201</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A42" s="1" t="s">
-        <v>131</v>
+        <v>88</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>136</v>
+        <v>86</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>135</v>
+        <v>87</v>
       </c>
       <c r="D42" s="1" t="s">
-        <v>134</v>
+        <v>90</v>
       </c>
       <c r="E42" s="1" t="s">
-        <v>132</v>
+        <v>89</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A43" s="1" t="s">
-        <v>172</v>
+        <v>131</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>171</v>
+        <v>136</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>170</v>
+        <v>135</v>
       </c>
       <c r="D43" s="1" t="s">
-        <v>176</v>
+        <v>134</v>
       </c>
       <c r="E43" s="1" t="s">
-        <v>173</v>
+        <v>132</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A44" s="1" t="s">
-        <v>192</v>
+        <v>172</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>193</v>
+        <v>171</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>194</v>
+        <v>170</v>
       </c>
       <c r="D44" s="1" t="s">
-        <v>195</v>
+        <v>176</v>
       </c>
       <c r="E44" s="1" t="s">
-        <v>196</v>
+        <v>173</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A45" s="1" t="s">
+        <v>192</v>
+      </c>
+      <c r="B45" s="1" t="s">
+        <v>193</v>
+      </c>
+      <c r="C45" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="D45" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="E45" s="1" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A46" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="B45" s="1" t="s">
+      <c r="B46" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="C45" s="1" t="s">
+      <c r="C46" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="D45" s="1" t="s">
+      <c r="D46" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="E45" s="1" t="s">
+      <c r="E46" s="1" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A46" s="2" t="s">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A47" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="B46" s="1" t="s">
+      <c r="B47" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="C46" s="2" t="s">
+      <c r="C47" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="D46" s="2" t="s">
+      <c r="D47" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="E46" s="2" t="s">
+      <c r="E47" s="2" t="s">
         <v>75</v>
       </c>
     </row>

</xml_diff>

<commit_message>
adding Kosuri et al
</commit_message>
<xml_diff>
--- a/primary_literature/TOC.xlsx
+++ b/primary_literature/TOC.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Shockwing/Dropbox/Boston/phd/repos/dnadesign-data/primary_literature/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2474378D-B4B7-0F46-935E-DEF3468510BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF62F56D-4114-1648-9905-CEE91CCE0A9C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17860" xr2:uid="{84B45C76-4322-224B-B312-91E503F65D31}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="235" uniqueCount="215">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="240" uniqueCount="220">
   <si>
     <t>comments</t>
   </si>
@@ -681,6 +681,21 @@
   </si>
   <si>
     <t>Deter et al. generated RNA-seq data on both antibiotic-treated and -untreated populations emerging from stationary phase.</t>
+  </si>
+  <si>
+    <t>Composability of regulatory sequences controlling transcription and translation in Escherichia coli</t>
+  </si>
+  <si>
+    <t>Kosuri et al</t>
+  </si>
+  <si>
+    <t>10.1073/pnas.1301301110</t>
+  </si>
+  <si>
+    <t>Promoter engineering</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kosuri et al. synthesized 12,563 combinations of common promoters and ribosome binding sites and simultaneously measured DNA, RNA, and protein levels from the entire library. </t>
   </si>
 </sst>
 </file>
@@ -1046,10 +1061,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{84F68783-878B-3345-9072-70C5BAEE55D7}">
-  <dimension ref="A1:E47"/>
+  <dimension ref="A1:E48"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C30" sqref="C30"/>
+    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1399,461 +1414,478 @@
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A21" s="2" t="s">
+      <c r="A21" s="1" t="s">
+        <v>216</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>215</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>217</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>218</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A22" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B21" s="2" t="s">
+      <c r="B22" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="C21" s="2" t="s">
+      <c r="C22" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="D21" s="2" t="s">
+      <c r="D22" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="E21" s="2" t="s">
+      <c r="E22" s="2" t="s">
         <v>11</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A22" s="1" t="s">
-        <v>181</v>
-      </c>
-      <c r="B22" s="1" t="s">
-        <v>179</v>
-      </c>
-      <c r="C22" s="1" t="s">
-        <v>180</v>
-      </c>
-      <c r="D22" s="1" t="s">
-        <v>176</v>
-      </c>
-      <c r="E22" s="1" t="s">
-        <v>182</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
-        <v>38</v>
+        <v>181</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>34</v>
+        <v>179</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>37</v>
+        <v>180</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>35</v>
+        <v>176</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>36</v>
+        <v>182</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
-        <v>151</v>
+        <v>38</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>152</v>
+        <v>34</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>153</v>
+        <v>37</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>154</v>
+        <v>35</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>155</v>
+        <v>36</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
-        <v>51</v>
+        <v>151</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>47</v>
+        <v>152</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>50</v>
+        <v>153</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>48</v>
+        <v>154</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>49</v>
+        <v>155</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
-        <v>206</v>
+        <v>51</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>207</v>
+        <v>47</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>208</v>
+        <v>50</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>20</v>
+        <v>48</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>209</v>
+        <v>49</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="s">
-        <v>105</v>
+        <v>206</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>109</v>
+        <v>207</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>108</v>
+        <v>208</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>106</v>
+        <v>20</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>107</v>
+        <v>209</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A28" s="1" t="s">
-        <v>69</v>
+        <v>105</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>66</v>
+        <v>109</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>68</v>
+        <v>108</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>58</v>
+        <v>106</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>67</v>
+        <v>107</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A29" s="1" t="s">
-        <v>65</v>
+        <v>69</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>64</v>
+        <v>68</v>
       </c>
       <c r="D29" s="1" t="s">
         <v>58</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>63</v>
+        <v>67</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A30" s="1" t="s">
-        <v>61</v>
+        <v>65</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>57</v>
+        <v>62</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="D30" s="1" t="s">
         <v>58</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A31" s="1" t="s">
-        <v>46</v>
+        <v>61</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>43</v>
+        <v>57</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>45</v>
+        <v>60</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>28</v>
+        <v>58</v>
       </c>
       <c r="E31" s="1" t="s">
-        <v>44</v>
+        <v>59</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A32" s="1" t="s">
-        <v>147</v>
+        <v>46</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>148</v>
+        <v>43</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>149</v>
+        <v>45</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>20</v>
+        <v>28</v>
       </c>
       <c r="E32" s="1" t="s">
-        <v>150</v>
+        <v>44</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A33" s="1" t="s">
-        <v>161</v>
+        <v>147</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>162</v>
+        <v>148</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>163</v>
+        <v>149</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>141</v>
+        <v>20</v>
       </c>
       <c r="E33" s="1" t="s">
-        <v>164</v>
+        <v>150</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A34" s="1" t="s">
-        <v>96</v>
+        <v>161</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>99</v>
+        <v>162</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>98</v>
+        <v>163</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>20</v>
+        <v>141</v>
       </c>
       <c r="E34" s="1" t="s">
-        <v>97</v>
+        <v>164</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A35" s="1" t="s">
-        <v>127</v>
+        <v>96</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>128</v>
+        <v>99</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>133</v>
+        <v>98</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>129</v>
+        <v>20</v>
       </c>
       <c r="E35" s="1" t="s">
-        <v>130</v>
+        <v>97</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A36" s="1" t="s">
-        <v>100</v>
+        <v>127</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>104</v>
+        <v>128</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>103</v>
+        <v>133</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>101</v>
+        <v>129</v>
       </c>
       <c r="E36" s="1" t="s">
-        <v>102</v>
+        <v>130</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A37" s="1" t="s">
-        <v>143</v>
+        <v>100</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>144</v>
+        <v>104</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>145</v>
+        <v>103</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>112</v>
+        <v>101</v>
       </c>
       <c r="E37" s="1" t="s">
-        <v>146</v>
+        <v>102</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A38" s="1" t="s">
-        <v>95</v>
+        <v>143</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>91</v>
+        <v>144</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>92</v>
+        <v>145</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>93</v>
+        <v>112</v>
       </c>
       <c r="E38" s="1" t="s">
-        <v>94</v>
+        <v>146</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A39" s="1" t="s">
-        <v>33</v>
+        <v>95</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>30</v>
+        <v>91</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>32</v>
+        <v>92</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>20</v>
+        <v>93</v>
       </c>
       <c r="E39" s="1" t="s">
-        <v>31</v>
+        <v>94</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A40" s="1" t="s">
-        <v>178</v>
+        <v>33</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>174</v>
+        <v>30</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>175</v>
+        <v>32</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>176</v>
+        <v>20</v>
       </c>
       <c r="E40" s="1" t="s">
-        <v>177</v>
+        <v>31</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A41" s="1" t="s">
-        <v>197</v>
+        <v>178</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>198</v>
+        <v>174</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>199</v>
+        <v>175</v>
       </c>
       <c r="D41" s="1" t="s">
-        <v>200</v>
+        <v>176</v>
       </c>
       <c r="E41" s="1" t="s">
-        <v>201</v>
+        <v>177</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A42" s="1" t="s">
-        <v>88</v>
+        <v>197</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>86</v>
+        <v>198</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>87</v>
+        <v>199</v>
       </c>
       <c r="D42" s="1" t="s">
-        <v>90</v>
+        <v>200</v>
       </c>
       <c r="E42" s="1" t="s">
-        <v>89</v>
+        <v>201</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A43" s="1" t="s">
-        <v>131</v>
+        <v>88</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>136</v>
+        <v>86</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>135</v>
+        <v>87</v>
       </c>
       <c r="D43" s="1" t="s">
-        <v>134</v>
+        <v>90</v>
       </c>
       <c r="E43" s="1" t="s">
-        <v>132</v>
+        <v>89</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A44" s="1" t="s">
-        <v>172</v>
+        <v>131</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>171</v>
+        <v>136</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>170</v>
+        <v>135</v>
       </c>
       <c r="D44" s="1" t="s">
-        <v>176</v>
+        <v>134</v>
       </c>
       <c r="E44" s="1" t="s">
-        <v>173</v>
+        <v>132</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A45" s="1" t="s">
-        <v>192</v>
+        <v>172</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>193</v>
+        <v>171</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>194</v>
+        <v>170</v>
       </c>
       <c r="D45" s="1" t="s">
-        <v>195</v>
+        <v>176</v>
       </c>
       <c r="E45" s="1" t="s">
-        <v>196</v>
+        <v>173</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A46" s="1" t="s">
+        <v>192</v>
+      </c>
+      <c r="B46" s="1" t="s">
+        <v>193</v>
+      </c>
+      <c r="C46" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="D46" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="E46" s="1" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A47" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="B46" s="1" t="s">
+      <c r="B47" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="C46" s="1" t="s">
+      <c r="C47" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="D46" s="1" t="s">
+      <c r="D47" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="E46" s="1" t="s">
+      <c r="E47" s="1" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A47" s="2" t="s">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A48" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="B47" s="1" t="s">
+      <c r="B48" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="C47" s="2" t="s">
+      <c r="C48" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="D47" s="2" t="s">
+      <c r="D48" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="E47" s="2" t="s">
+      <c r="E48" s="2" t="s">
         <v>75</v>
       </c>
     </row>

</xml_diff>